<commit_message>
Operation sheet of funding system
and some reference to design
</commit_message>
<xml_diff>
--- a/Documents/ProductBacklog_Team_apocalypse.xlsx
+++ b/Documents/ProductBacklog_Team_apocalypse.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles\Dropbox\ICT1\Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="19440" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="19440" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Product_Backlog" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -19,7 +24,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="A11" authorId="0">
+    <comment ref="A11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -32,7 +37,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B11" authorId="0">
+    <comment ref="B11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -46,7 +51,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C11" authorId="0">
+    <comment ref="C11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -60,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E11" authorId="0">
+    <comment ref="E11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -79,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="88">
   <si>
     <t>Story ID</t>
   </si>
@@ -141,12 +146,6 @@
     <t>Requirement Analysis</t>
   </si>
   <si>
-    <t>Payment Portal</t>
-  </si>
-  <si>
-    <t>Designing layout</t>
-  </si>
-  <si>
     <t>Unit Testing of registration functionality</t>
   </si>
   <si>
@@ -174,9 +173,6 @@
     <t>Email subscription</t>
   </si>
   <si>
-    <t>Adding dropdown to the search categories</t>
-  </si>
-  <si>
     <t>Functionality to edit [add, modify, delete] user profile</t>
   </si>
   <si>
@@ -189,17 +185,7 @@
     <t>User Registration: Sign-In</t>
   </si>
   <si>
-    <t>Creating user packages</t>
-  </si>
-  <si>
     <t xml:space="preserve">Conducting kick-off meeting and subsequent meetings with client to get in depth idea about the project. Thourough analysis of the requirements from implementation perspective. </t>
-  </si>
-  <si>
-    <t>Need to add the dropdowns for search engine UI with specific categories. All values of the dropdown boxex should be read from database. 
-Inter-dependency of the drop-down values should be taken care. Ex. If the 'Country' has been selected as 'Malysia' then drop down for 'State' should have list of states from Malysia only. [Use JQuery or Ajax]</t>
-  </si>
-  <si>
-    <t>Finalize the template as per the discussion with Ms. Ping and team.  [Refer the layout sketch shared by Ms. Ping ]. Choosen template should satidfy all requirements mentioned by client.  Get go ahead from client on finalized template.</t>
   </si>
   <si>
     <t>Create sign-up page with multiple steps (Basic information, packages available etc). Include 'terms and conditions'  checkbox. 
@@ -237,9 +223,6 @@
 d) User ID entered is unique</t>
   </si>
   <si>
-    <t>Create main menu of the website with tabs home, Investor, Entrepreneur, About US, Contact etc. Also, create the sub-menu and devise and implement the navigation strategy considering whether the link should open in same or new window.</t>
-  </si>
-  <si>
     <t>Get confirmation from client on various sections and sub-sections of the home page.
 Collect the contents for all of the finalized sections. Arrange it on the home page appropriately.</t>
   </si>
@@ -251,18 +234,6 @@
   </si>
   <si>
     <t>Currently, only reset password functionality is present. Provide a 'Forgot Password' feature which would ask 'DOB' and some secret question and would send auto generated password to registered e-mail account.</t>
-  </si>
-  <si>
-    <t>Creating packages for the users based on the services offered. 
-Three packages which need to be created are:
-1) Free: No fee for this account. 
-Only outline of the BP will be available to other users.
-2) Pro: S$ 99. 
-Details of the BP woud be made avaialable to first 10 users. 
-User would be required to recharge again to make his/her BP visible to others.
-3) Global Pro: S$199
-Details of the BP woud be made avaialable to first 40 users. 
-User would be required to recharge again to make his/her BP visible to others.</t>
   </si>
   <si>
     <t>Create sign-in page which will accept UserID and password of the registered user. 
@@ -283,7 +254,121 @@
     <t>Ming Qian Li</t>
   </si>
   <si>
-    <t>Athena Wang</t>
+    <t>Distinguish several functions(Entrepreneur, Information, Sub Websites)</t>
+  </si>
+  <si>
+    <t>Task need to separate as main functionial systems, crowd funding, information and subwebsite systems 
+Inter-dependency of the drop-down values should be taken care. Ex. If the 'Country' has been selected as 'Malysia' then drop down for 'State' should have list of states from Malysia only. [Use JQuery or Ajax]</t>
+  </si>
+  <si>
+    <t>Designing layout and check out with client</t>
+  </si>
+  <si>
+    <t>According to the prototype which client decided, to finish design and layout. To meet the client again and checkout</t>
+  </si>
+  <si>
+    <t>Payment Portal for crowd funding system</t>
+  </si>
+  <si>
+    <t>Creating user own website</t>
+  </si>
+  <si>
+    <t>Creating website for the users based on the multisites funcitons. 
+1, User can choose the template installed perviously
+2, User can design and develop it again
+3, User can post contents include pictures, videos and journals</t>
+  </si>
+  <si>
+    <t>Creating the project categories and information categories</t>
+  </si>
+  <si>
+    <t>Create main menu of the website with tabs home, project, business competition, About US, Contact etc. Also, create the sub-menu and devise and implement the navigation strategy considering whether the link should open in same or new window.</t>
+  </si>
+  <si>
+    <t>Obtain the details from client again, to settle up the categories for projects and business informations</t>
+  </si>
+  <si>
+    <t>User own project publish function</t>
+  </si>
+  <si>
+    <t>User can publish their project, prodcuts or ideas from homepage</t>
+  </si>
+  <si>
+    <t>User own website interface</t>
+  </si>
+  <si>
+    <t>User can have their own dashboard for their website</t>
+  </si>
+  <si>
+    <t>the each client project must be tested properly to certain their space, domain-name and the other things can work normally</t>
+  </si>
+  <si>
+    <t>Sub-system balance adjustment</t>
+  </si>
+  <si>
+    <t>Social meida count</t>
+  </si>
+  <si>
+    <t>the social media count functon must be implement differently in main site and customers sites.</t>
+  </si>
+  <si>
+    <t>backup functions to database</t>
+  </si>
+  <si>
+    <t>backup functions to whole website</t>
+  </si>
+  <si>
+    <t>Commerical module for subsite</t>
+  </si>
+  <si>
+    <t>customized silder of sub-sites</t>
+  </si>
+  <si>
+    <t>Share the like to the social media</t>
+  </si>
+  <si>
+    <t>Login with social media account</t>
+  </si>
+  <si>
+    <t>Burgeen.com Project Team</t>
+  </si>
+  <si>
+    <t>final result adjustment</t>
+  </si>
+  <si>
+    <t>prepareation of deliverable process</t>
+  </si>
+  <si>
+    <t>to backup the data from the whole website, both the main sites and sub-sites</t>
+  </si>
+  <si>
+    <t>to backup the files from the whole website, all the contents including pictures and videos.</t>
+  </si>
+  <si>
+    <t>the module for the customers who want ot create the shopping mall or the other commerce websites</t>
+  </si>
+  <si>
+    <t>the function to enable customers who can create their own silder to demonstrate</t>
+  </si>
+  <si>
+    <t>the function to enable customers who can share their like from website to social media</t>
+  </si>
+  <si>
+    <t>the function to enable user can login the platform using their social media accounts</t>
+  </si>
+  <si>
+    <t>Arrange the related links</t>
+  </si>
+  <si>
+    <t>add more related links to platform</t>
+  </si>
+  <si>
+    <t xml:space="preserve">including:copyright declaration
+IP declaration
+</t>
+  </si>
+  <si>
+    <t>presentation and demonstartiong to client</t>
   </si>
 </sst>
 </file>
@@ -616,6 +701,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -663,7 +751,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -698,7 +786,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -907,25 +995,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="24" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" style="25" customWidth="1"/>
-    <col min="3" max="3" width="76.5703125" style="25" customWidth="1"/>
-    <col min="4" max="4" width="26.7109375" style="25" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" style="24" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" style="25" customWidth="1"/>
+    <col min="3" max="3" width="76.5546875" style="25" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" style="25" customWidth="1"/>
     <col min="5" max="5" width="14" style="24" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" style="24" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" style="25" customWidth="1"/>
-    <col min="8" max="16384" width="9.85546875" style="3"/>
+    <col min="6" max="6" width="17.88671875" style="24" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" style="25" customWidth="1"/>
+    <col min="8" max="16384" width="9.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -934,7 +1022,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="30" t="s">
         <v>13</v>
       </c>
@@ -945,7 +1033,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -954,13 +1042,13 @@
       <c r="F3" s="5"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6"/>
       <c r="B4" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="10"/>
@@ -971,13 +1059,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="B5" s="7" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="10"/>
@@ -988,13 +1076,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
       <c r="B6" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="10"/>
@@ -1005,13 +1093,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6"/>
       <c r="B7" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="10"/>
@@ -1022,20 +1110,20 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
       <c r="B8" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="1"/>
       <c r="F8" s="19"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="20"/>
       <c r="C9" s="20"/>
@@ -1044,7 +1132,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="21"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1053,7 +1141,7 @@
       <c r="F10" s="21"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="s">
         <v>0</v>
       </c>
@@ -1076,7 +1164,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="23" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" s="23" customFormat="1" ht="43.2" x14ac:dyDescent="0.25">
       <c r="A12" s="27">
         <v>1</v>
       </c>
@@ -1084,7 +1172,7 @@
         <v>19</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D12" s="27"/>
       <c r="E12" s="27" t="s">
@@ -1095,15 +1183,15 @@
       </c>
       <c r="G12" s="27"/>
     </row>
-    <row r="13" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" s="27">
         <v>2</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="D13" s="27"/>
       <c r="E13" s="27" t="s">
@@ -1114,15 +1202,15 @@
       </c>
       <c r="G13" s="27"/>
     </row>
-    <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="27">
         <v>3</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="D14" s="27"/>
       <c r="E14" s="27" t="s">
@@ -1133,15 +1221,15 @@
       </c>
       <c r="G14" s="27"/>
     </row>
-    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="27">
         <v>4</v>
       </c>
       <c r="B15" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="28" t="s">
         <v>34</v>
-      </c>
-      <c r="C15" s="28" t="s">
-        <v>40</v>
       </c>
       <c r="D15" s="27"/>
       <c r="E15" s="27" t="s">
@@ -1152,32 +1240,34 @@
       </c>
       <c r="G15" s="27"/>
     </row>
-    <row r="16" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="27">
         <v>5</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
+      <c r="E16" s="27" t="s">
+        <v>7</v>
+      </c>
       <c r="F16" s="27" t="s">
         <v>8</v>
       </c>
       <c r="G16" s="27"/>
     </row>
-    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" s="27">
         <v>6</v>
       </c>
-      <c r="B17" s="27" t="s">
-        <v>20</v>
+      <c r="B17" s="28" t="s">
+        <v>55</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D17" s="27"/>
       <c r="E17" s="27" t="s">
@@ -1188,15 +1278,15 @@
       </c>
       <c r="G17" s="27"/>
     </row>
-    <row r="18" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="27">
         <v>7</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D18" s="27"/>
       <c r="E18" s="27" t="s">
@@ -1207,15 +1297,15 @@
       </c>
       <c r="G18" s="27"/>
     </row>
-    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="27">
         <v>8</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D19" s="27"/>
       <c r="E19" s="27" t="s">
@@ -1226,15 +1316,15 @@
       </c>
       <c r="G19" s="27"/>
     </row>
-    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="27">
         <v>9</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D20" s="27"/>
       <c r="E20" s="27" t="s">
@@ -1245,15 +1335,15 @@
       </c>
       <c r="G20" s="27"/>
     </row>
-    <row r="21" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="27">
         <v>10</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D21" s="27"/>
       <c r="E21" s="27" t="s">
@@ -1264,15 +1354,15 @@
       </c>
       <c r="G21" s="27"/>
     </row>
-    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="27">
         <v>11</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D22" s="27"/>
       <c r="E22" s="27" t="s">
@@ -1283,15 +1373,15 @@
       </c>
       <c r="G22" s="27"/>
     </row>
-    <row r="23" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A23" s="27">
         <v>12</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D23" s="27"/>
       <c r="E23" s="27" t="s">
@@ -1302,15 +1392,15 @@
       </c>
       <c r="G23" s="27"/>
     </row>
-    <row r="24" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="27">
         <v>13</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="D24" s="27"/>
       <c r="E24" s="27" t="s">
@@ -1321,15 +1411,15 @@
       </c>
       <c r="G24" s="27"/>
     </row>
-    <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="27">
         <v>14</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D25" s="27"/>
       <c r="E25" s="27" t="s">
@@ -1340,15 +1430,15 @@
       </c>
       <c r="G25" s="27"/>
     </row>
-    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="27">
         <v>15</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C26" s="28" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D26" s="27"/>
       <c r="E26" s="27" t="s">
@@ -1359,15 +1449,15 @@
       </c>
       <c r="G26" s="27"/>
     </row>
-    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" s="27">
         <v>16</v>
       </c>
       <c r="B27" s="28" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C27" s="28" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D27" s="27"/>
       <c r="E27" s="27" t="s">
@@ -1378,15 +1468,15 @@
       </c>
       <c r="G27" s="27"/>
     </row>
-    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" s="27">
         <v>17</v>
       </c>
       <c r="B28" s="29" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D28" s="27"/>
       <c r="E28" s="27" t="s">
@@ -1397,15 +1487,15 @@
       </c>
       <c r="G28" s="27"/>
     </row>
-    <row r="29" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A29" s="27">
         <v>18</v>
       </c>
       <c r="B29" s="28" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D29" s="27"/>
       <c r="E29" s="27" t="s">
@@ -1415,6 +1505,257 @@
         <v>8</v>
       </c>
       <c r="G29" s="27"/>
+    </row>
+    <row r="30" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="27">
+        <v>19</v>
+      </c>
+      <c r="B30" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+    </row>
+    <row r="31" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="27">
+        <v>20</v>
+      </c>
+      <c r="B31" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="27">
+        <v>21</v>
+      </c>
+      <c r="B32" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="27"/>
+      <c r="G32" s="27"/>
+    </row>
+    <row r="33" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="27">
+        <v>22</v>
+      </c>
+      <c r="B33" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" s="27"/>
+      <c r="G33" s="27"/>
+    </row>
+    <row r="34" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="27">
+        <v>23</v>
+      </c>
+      <c r="B34" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="27"/>
+      <c r="G34" s="27"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="27">
+        <v>24</v>
+      </c>
+      <c r="B35" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="D35" s="27"/>
+      <c r="E35" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35" s="27"/>
+      <c r="G35" s="27"/>
+    </row>
+    <row r="36" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="27">
+        <v>25</v>
+      </c>
+      <c r="B36" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="D36" s="27"/>
+      <c r="E36" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="G36" s="27"/>
+    </row>
+    <row r="37" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="27">
+        <v>26</v>
+      </c>
+      <c r="B37" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F37" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="G37" s="27"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="27">
+        <v>27</v>
+      </c>
+      <c r="B38" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="C38" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="D38" s="27"/>
+      <c r="E38" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="27"/>
+      <c r="G38" s="27"/>
+    </row>
+    <row r="39" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="27">
+        <v>29</v>
+      </c>
+      <c r="B39" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="C39" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="27"/>
+      <c r="G39" s="27"/>
+    </row>
+    <row r="40" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="27">
+        <v>30</v>
+      </c>
+      <c r="B40" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="C40" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="27">
+        <v>31</v>
+      </c>
+      <c r="B41" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="C41" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="D41" s="27"/>
+      <c r="E41" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41" s="27"/>
+      <c r="G41" s="27"/>
+    </row>
+    <row r="42" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A42" s="27">
+        <v>33</v>
+      </c>
+      <c r="B42" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="C42" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="D42" s="27"/>
+      <c r="E42" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F42" s="27"/>
+      <c r="G42" s="27"/>
+    </row>
+    <row r="43" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A43" s="27">
+        <v>34</v>
+      </c>
+      <c r="B43" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="C43" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="D43" s="27"/>
+      <c r="E43" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" s="27"/>
+      <c r="G43" s="27"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" s="27"/>
+      <c r="B44" s="28"/>
+      <c r="C44" s="28"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="27"/>
+      <c r="F44" s="27"/>
+      <c r="G44" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>